<commit_message>
Build v2.1.2: Fix SearchCriteria variants and Schemas sheet grouping/sorting
</commit_message>
<xml_diff>
--- a/Templates Converted/amendChangeSettlementBIC.230511.xlsx
+++ b/Templates Converted/amendChangeSettlementBIC.230511.xlsx
@@ -743,7 +743,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -872,6 +872,43 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>content</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -885,7 +922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1014,6 +1051,43 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>content</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -1027,7 +1101,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScale="81" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
@@ -1167,630 +1241,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dateTime</t>
+          <t>amendChangeSettlementBIC.230511Request</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>The date and time of the API Request creation</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>schema</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>amendChangeSettlementBIC.230511Request</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>YYYY-MM-DDTHH:MM:SS[.M{1,6}]</t>
-        </is>
-      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2019-06-21T23:20:50.000001; 2024-11-08T14:29:00.012345; 9999-12-31T12:55:45.000001</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>settlementBIC</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>settlementBICCode</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>settlementBIC</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>The Settlement BIC adhering to CGS. This is the settlement BIC of the STEP2 DP Preferred Agent in the relevant Step2 service.</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Bic11Only</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>4!c2!a2!c3!c</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>IPSDID21XXX; TESBIC11XXX; TESBIC99XXX</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>initialSettBICValidityDate</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>settlementBIC</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>The Initial Parameter Validity Date set in the original command to be amended.</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>YYYY-MM-DD</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>2019-06-21; 2024-11-08; 9999-12-31</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>endSettBICValidityDate</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>settlementBIC</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>The End Parameter Validity Date set in the original command to be amended.</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>YYYY-MM-DD</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>2019-06-21; 2024-11-08; 9999-12-31</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>settlementBICAmend</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>settlBICName</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>settlementBICAmend</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>The name of the Settlement BIC</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>ParticipantName</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>ExampleBank01; ExampleBank02; ExampleBank03</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>automaticAdjustment</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>settlementBICAmend</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>This parameter indicates if the Settlement BIC opts out of the automatic liquidity adjustments performed by the module at the EOL. In this case, thresholds are configured only to trigger alerts</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Boolean</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>true; false</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>eodFulDefund</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>settlementBICAmend</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>This parameter indicates if the Settlement BIC opts for the CGS to perform an automatic full defunding of the Settlement BIC position on the last LAC of the business day in order to avoid remuneration of outstanding liquidity</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Boolean</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>true; false</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>lmrFileRequired</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>settlementBICAmend</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>This parameter indicates whether the Settlement BIC must be configured to receive the LMR output file</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Boolean</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>true; false</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>lnrFileRequired</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>settlementBICAmend</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>This parameter indicates whether the Settlement BIC must be configured to receive the LNR output file</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Boolean</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>true; false</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>dlrFileRequired</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>settlementBICAmend</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>This parameter indicates whether the Settlement BIC must be configured to receive daily liquidity reconciliation report</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Boolean</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>true; false</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>body</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>maxRcvgFileSize</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>settlementBICAmend</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>The maximum size of an output file generated and sent by the CGS to the Settlement BIC</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Number</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>999999999999999</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>100000; 99999999999999; 1</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1 D3:D1048576">
@@ -1873,7 +1351,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2010,87 +1488,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dateTime</t>
+          <t>amendChangeSettlementBIC.230511Response</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>The date and time of the API Response creation</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>schema</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>amendChangeSettlementBIC.230511Response</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>YYYY-MM-DDTHH:MM:SS[.M{1,6}]</t>
-        </is>
-      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2019-06-21T23:20:50.000001; 2024-11-08T14:29:00.012345; 9999-12-31T12:55:45.000001</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>content</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>commandRef</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>The command reference</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>F010190208113908; F011390508223918; F123456789012345</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2105,7 +1530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2234,6 +1659,43 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>content</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>amendChangeSettlementBIC.230511Response</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>amendChangeSettlementBIC.230511Response</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -2247,7 +1709,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2384,173 +1846,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dateTime</t>
+          <t>errorResponse</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>The date and time of the API Response creation</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>schema</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>errorResponse</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>YYYY-MM-DDTHH:MM:SS[.M{1,6}]</t>
-        </is>
-      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2019-06-21T23:20:50.000001; 2024-11-08T14:29:00.012345; 9999-12-31T12:55:45.000001</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>content</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>errorCode</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>The relevant error code</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>AX01; R01, XT92</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>content</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>errorCodeDescription</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>The description of the error</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>255</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Transaction rejected; File rejected; Schema error</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>content</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>requestId</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>The automatically generated identification of the API request</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>REQID000011112222333445661234567890; REQID000011112222333445661234567891; REQID000011112222333445661234567892</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2565,7 +1888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2694,6 +2017,43 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>content</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -2707,7 +2067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2836,6 +2196,43 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>content</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -2849,7 +2246,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2978,6 +2375,43 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>content</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>errorResponse1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>